<commit_message>
1. Excel TO JSon 讀取部分。
</commit_message>
<xml_diff>
--- a/Client/Assets/EventData.xlsx
+++ b/Client/Assets/EventData.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,7 +182,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>End</t>
+    <t>測試用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EOC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TstByte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestUINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testnon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0aa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -581,136 +641,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AK8"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView tabSelected="1" topLeftCell="P2" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="5" t="s">
-        <v>39</v>
+      <c r="AN2" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -808,16 +885,28 @@
       <c r="AJ3" t="s">
         <v>36</v>
       </c>
+      <c r="AK3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -915,29 +1004,184 @@
       <c r="AJ4" t="s">
         <v>38</v>
       </c>
+      <c r="AK4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>123</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>22</v>
+      </c>
+      <c r="L5">
+        <v>24</v>
+      </c>
+      <c r="M5">
+        <v>26</v>
+      </c>
+      <c r="N5">
+        <v>28</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>32</v>
+      </c>
+      <c r="Q5">
+        <v>34</v>
+      </c>
+      <c r="R5">
+        <v>36</v>
+      </c>
+      <c r="S5">
+        <v>38</v>
+      </c>
+      <c r="T5">
+        <v>40</v>
+      </c>
+      <c r="U5">
+        <v>42</v>
+      </c>
+      <c r="V5">
+        <v>44</v>
+      </c>
+      <c r="W5">
+        <v>46</v>
+      </c>
+      <c r="X5">
+        <v>48</v>
+      </c>
+      <c r="Y5">
+        <v>50</v>
+      </c>
+      <c r="Z5">
+        <v>52</v>
+      </c>
+      <c r="AA5">
+        <v>54</v>
+      </c>
+      <c r="AB5">
+        <v>56</v>
+      </c>
+      <c r="AC5">
+        <v>58</v>
+      </c>
+      <c r="AD5">
+        <v>60</v>
+      </c>
+      <c r="AE5">
+        <v>62</v>
+      </c>
+      <c r="AF5">
+        <v>64</v>
+      </c>
+      <c r="AG5">
+        <v>66</v>
+      </c>
+      <c r="AH5">
+        <v>68</v>
+      </c>
+      <c r="AI5">
+        <v>70</v>
+      </c>
+      <c r="AJ5">
+        <v>72</v>
+      </c>
+      <c r="AK5">
+        <v>74</v>
+      </c>
+      <c r="AL5">
+        <v>76</v>
+      </c>
+      <c r="AM5">
+        <v>78</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>123</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="O6">
+        <v>98</v>
+      </c>
+      <c r="R6">
+        <v>31</v>
+      </c>
+      <c r="U6">
+        <v>56465</v>
+      </c>
+      <c r="X6">
+        <v>12</v>
+      </c>
+      <c r="AA6">
+        <v>50</v>
+      </c>
+      <c r="AD6">
+        <v>1254</v>
+      </c>
+      <c r="AJ6">
+        <v>66</v>
+      </c>
+      <c r="AM6">
+        <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>